<commit_message>
Finish Mock HttpServer and Home Page (Draft Version)
Home Page TODO:
!! Redesign header part to make it responsive
!! Redesign footer part to make it responsive
!!Add Side pannel and make it shows on "< middle size screen"

(optional) Add an suitable background to the page.
</commit_message>
<xml_diff>
--- a/设计/需求分析.xlsx
+++ b/设计/需求分析.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\HummingBird\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\HummingBird\设计\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7277DF8E-1554-46F6-9841-7B56CA29AB79}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9756B02-93A0-460D-BB3A-D83AB01D04BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="总体需求" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
   <si>
     <t>分类</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -243,10 +243,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>按照筛选时筛选文章</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>每次只显示一个板块中的文章</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -267,10 +263,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>修改用户名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>修改用户密码时需要确认密码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -323,19 +315,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>列出所有分类</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>列出所有板块</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>修改板块名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>修改板块的背景颜色</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -434,6 +418,14 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出一个板块中的所有分类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看所有本地图片</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -888,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -965,10 +957,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
@@ -979,10 +971,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>20</v>
@@ -999,10 +991,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
@@ -1016,7 +1008,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>23</v>
@@ -1032,11 +1024,11 @@
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>15</v>
+      <c r="D9" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1047,7 +1039,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>61</v>
@@ -1058,277 +1050,264 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>63</v>
+        <v>95</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E14" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>81</v>
+      <c r="A37" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>40</v>
+      <c r="A39" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created axure rp prototype
</commit_message>
<xml_diff>
--- a/设计/需求分析.xlsx
+++ b/设计/需求分析.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\HummingBird\设计\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9756B02-93A0-460D-BB3A-D83AB01D04BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B27F6E2-63CA-434E-91F9-BF8B17CC926F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="总体需求" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="98">
   <si>
     <t>分类</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -426,6 +426,10 @@
   </si>
   <si>
     <t>查看所有本地图片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>为文章指定封面图片</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -880,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1256,58 +1260,63 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update prototype, finished article edtior, account setting page and 'about me' edit page
</commit_message>
<xml_diff>
--- a/设计/需求分析.xlsx
+++ b/设计/需求分析.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\HummingBird\设计\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B27F6E2-63CA-434E-91F9-BF8B17CC926F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EDE128-846B-4D27-A4ED-F946F78CEFB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="3435" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="总体需求" sheetId="1" r:id="rId1"/>
@@ -147,14 +147,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>能够添加列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>能够加粗、斜体</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>能够添加代码块（行内和块级别）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -164,10 +156,6 @@
   </si>
   <si>
     <t>能够高亮Java、JavaScript、Python、C和C++的代码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>能上传图片并将图片添加到文章中</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -430,6 +418,18 @@
   </si>
   <si>
     <t>为文章指定封面图片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>能够加粗、斜体、下划线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>能够添加列表（有序和无序）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -886,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -902,7 +902,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -935,13 +935,13 @@
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -961,10 +961,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
@@ -975,10 +975,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>20</v>
@@ -986,24 +986,24 @@
     </row>
     <row r="7" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>14</v>
@@ -1029,24 +1029,24 @@
         <v>10</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>21</v>
@@ -1054,54 +1054,54 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
@@ -1119,7 +1119,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1129,80 +1129,80 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
@@ -1210,7 +1210,7 @@
         <v>25</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1218,7 +1218,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1226,7 +1226,7 @@
         <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1234,55 +1234,55 @@
         <v>3</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1292,32 +1292,32 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update prototype, working on the image manage page.
</commit_message>
<xml_diff>
--- a/设计/需求分析.xlsx
+++ b/设计/需求分析.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\HummingBird\设计\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EDE128-846B-4D27-A4ED-F946F78CEFB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22ABED32-5563-46C9-A9AD-7F8FF470775C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="3435" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3255" yWindow="-270" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="总体需求" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="106">
   <si>
     <t>分类</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,10 +108,6 @@
   </si>
   <si>
     <t>新增图片</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>删除图片</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -430,6 +426,42 @@
   </si>
   <si>
     <t>能够添加列表（有序和无序）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新建图片分类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改图片分类名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将一张图片从一个分类移动到另一个分类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除图片分类，并将该分类中所有图片移动到未分类中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除图片分类，并将该分类中所有图片移动到用户指定的分类中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除图片分类，并删除该分类中的所有图片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一次删除一张图片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一次删除多张图片</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -886,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -902,7 +934,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -935,19 +967,19 @@
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -961,10 +993,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
@@ -975,10 +1007,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>20</v>
@@ -986,24 +1018,24 @@
     </row>
     <row r="7" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -1015,12 +1047,12 @@
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>14</v>
@@ -1029,204 +1061,228 @@
         <v>10</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>68</v>
+        <v>53</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>93</v>
+        <v>50</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C24" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="s">
         <v>78</v>
       </c>
-      <c r="C23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="6" t="s">
+    </row>
+    <row r="30" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1234,90 +1290,90 @@
         <v>3</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>